<commit_message>
final update on Apr.18
</commit_message>
<xml_diff>
--- a/Reports/Raw Data Spreadsheet.xlsx
+++ b/Reports/Raw Data Spreadsheet.xlsx
@@ -5,19 +5,21 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hyu/Documents/McMaster/CAS764/Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hyu/Documents/McMaster/CAS764/Project/Reports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3F9A69B-96C0-BD42-B2F5-1D257F243AB2}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93946434-FAD9-1E4F-B906-C98725C633D1}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="640" yWindow="460" windowWidth="19660" windowHeight="16140" activeTab="4" xr2:uid="{17E0CC5E-A7C5-2F4B-B0F5-FD8DEB8C59A4}"/>
+    <workbookView xWindow="640" yWindow="460" windowWidth="19660" windowHeight="16140" activeTab="6" xr2:uid="{17E0CC5E-A7C5-2F4B-B0F5-FD8DEB8C59A4}"/>
   </bookViews>
   <sheets>
     <sheet name="CONLL CNN" sheetId="1" r:id="rId1"/>
     <sheet name="CONLL RNN" sheetId="4" r:id="rId2"/>
     <sheet name="NEEL CNN" sheetId="2" r:id="rId3"/>
     <sheet name="NEEL RNN" sheetId="3" r:id="rId4"/>
-    <sheet name="Sheet2" sheetId="5" r:id="rId5"/>
+    <sheet name="CONLL HMM" sheetId="6" r:id="rId5"/>
+    <sheet name="Comparision" sheetId="5" r:id="rId6"/>
+    <sheet name="BootStrap" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -29,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="864" uniqueCount="107">
   <si>
     <t>CONLL CNN</t>
   </si>
@@ -194,6 +196,162 @@
   </si>
   <si>
     <t>0H:3M:31S</t>
+  </si>
+  <si>
+    <t>CONLL HMM</t>
+  </si>
+  <si>
+    <t>0H:0M:35S</t>
+  </si>
+  <si>
+    <t>NEEL HMM</t>
+  </si>
+  <si>
+    <t>HMM</t>
+  </si>
+  <si>
+    <t>$byClass</t>
+  </si>
+  <si>
+    <t>2018-04-15 20:12:58 EDT</t>
+  </si>
+  <si>
+    <t>2018-04-15 20:13:33 EDT</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>Confusion</t>
+  </si>
+  <si>
+    <t>Matrix</t>
+  </si>
+  <si>
+    <t>and</t>
+  </si>
+  <si>
+    <t>Statistics</t>
+  </si>
+  <si>
+    <t>Overall</t>
+  </si>
+  <si>
+    <t>Accuracy</t>
+  </si>
+  <si>
+    <t>:</t>
+  </si>
+  <si>
+    <t>CI</t>
+  </si>
+  <si>
+    <t>(0.949,</t>
+  </si>
+  <si>
+    <t>0.9528)</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Information</t>
+  </si>
+  <si>
+    <t>Rate</t>
+  </si>
+  <si>
+    <t>P-Value</t>
+  </si>
+  <si>
+    <t>[Acc</t>
+  </si>
+  <si>
+    <t>NIR]</t>
+  </si>
+  <si>
+    <t>&lt;</t>
+  </si>
+  <si>
+    <t>Kappa</t>
+  </si>
+  <si>
+    <t>Mcnemar's</t>
+  </si>
+  <si>
+    <t>by</t>
+  </si>
+  <si>
+    <t>Sensitivity</t>
+  </si>
+  <si>
+    <t>Specificity</t>
+  </si>
+  <si>
+    <t>Pos</t>
+  </si>
+  <si>
+    <t>Pred</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Neg</t>
+  </si>
+  <si>
+    <t>Prevalence</t>
+  </si>
+  <si>
+    <t>Detection</t>
+  </si>
+  <si>
+    <t>Balanced</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>(0.9233,</t>
+  </si>
+  <si>
+    <t>0.928)</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>(0.8972,</t>
+  </si>
+  <si>
+    <t>1)</t>
+  </si>
+  <si>
+    <t>Table 1: Precision, Recall and F1 score of the three algorithms on two datasets.</t>
+  </si>
+  <si>
+    <t>Table 2: NER Classifier Consolidation</t>
+  </si>
+  <si>
+    <t>BEFORE</t>
+  </si>
+  <si>
+    <t>AFTER</t>
+  </si>
+  <si>
+    <t>CNN</t>
+  </si>
+  <si>
+    <t>BASELINE</t>
+  </si>
+  <si>
+    <t>BOOTSTRAP</t>
+  </si>
+  <si>
+    <t>Table 3: Baseline and Bootstrap Prediction Accuracy</t>
   </si>
 </sst>
 </file>
@@ -204,7 +362,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -219,8 +377,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -263,8 +433,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -272,12 +460,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -295,35 +498,86 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2696,7 +2950,7 @@
   <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView topLeftCell="B3" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:E30"/>
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3760,11 +4014,2394 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D81BBF1-2A54-344B-966E-6245C2B54D30}">
+  <dimension ref="A1:L139"/>
+  <sheetViews>
+    <sheetView topLeftCell="A107" workbookViewId="0">
+      <selection activeCell="I129" sqref="I129:I133"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8">
+        <v>42828</v>
+      </c>
+      <c r="D8">
+        <v>240</v>
+      </c>
+      <c r="E8">
+        <v>228</v>
+      </c>
+      <c r="F8">
+        <v>425</v>
+      </c>
+      <c r="G8">
+        <v>1052</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9">
+        <v>13</v>
+      </c>
+      <c r="D9">
+        <v>1720</v>
+      </c>
+      <c r="E9">
+        <v>23</v>
+      </c>
+      <c r="F9">
+        <v>119</v>
+      </c>
+      <c r="G9">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10">
+        <v>40</v>
+      </c>
+      <c r="D10">
+        <v>12</v>
+      </c>
+      <c r="E10">
+        <v>976</v>
+      </c>
+      <c r="F10">
+        <v>37</v>
+      </c>
+      <c r="G10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11">
+        <v>79</v>
+      </c>
+      <c r="D11">
+        <v>104</v>
+      </c>
+      <c r="E11">
+        <v>31</v>
+      </c>
+      <c r="F11">
+        <v>1479</v>
+      </c>
+      <c r="G11">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12">
+        <v>18</v>
+      </c>
+      <c r="D12">
+        <v>18</v>
+      </c>
+      <c r="E12">
+        <v>10</v>
+      </c>
+      <c r="F12">
+        <v>32</v>
+      </c>
+      <c r="G12">
+        <v>2042</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>68</v>
+      </c>
+      <c r="B14" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>69</v>
+      </c>
+      <c r="C16" t="s">
+        <v>70</v>
+      </c>
+      <c r="D16">
+        <v>0.95089999999999997</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B17" s="9">
+        <v>0.95</v>
+      </c>
+      <c r="C17" t="s">
+        <v>71</v>
+      </c>
+      <c r="D17" t="s">
+        <v>70</v>
+      </c>
+      <c r="E17" t="s">
+        <v>72</v>
+      </c>
+      <c r="F17" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>74</v>
+      </c>
+      <c r="C18" t="s">
+        <v>75</v>
+      </c>
+      <c r="D18" t="s">
+        <v>76</v>
+      </c>
+      <c r="E18" t="s">
+        <v>70</v>
+      </c>
+      <c r="F18">
+        <v>0.83330000000000004</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>77</v>
+      </c>
+      <c r="C19" t="s">
+        <v>78</v>
+      </c>
+      <c r="D19" t="s">
+        <v>21</v>
+      </c>
+      <c r="E19" t="s">
+        <v>79</v>
+      </c>
+      <c r="F19" t="s">
+        <v>70</v>
+      </c>
+      <c r="G19" t="s">
+        <v>80</v>
+      </c>
+      <c r="H19" s="10">
+        <v>2.2E-16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>81</v>
+      </c>
+      <c r="C21" t="s">
+        <v>70</v>
+      </c>
+      <c r="D21">
+        <v>0.81869999999999998</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
+        <v>82</v>
+      </c>
+      <c r="C22" t="s">
+        <v>29</v>
+      </c>
+      <c r="D22" t="s">
+        <v>77</v>
+      </c>
+      <c r="E22" t="s">
+        <v>70</v>
+      </c>
+      <c r="F22" t="s">
+        <v>80</v>
+      </c>
+      <c r="G22" s="10">
+        <v>2.2E-16</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>67</v>
+      </c>
+      <c r="B24" t="s">
+        <v>83</v>
+      </c>
+      <c r="C24" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
+        <v>16</v>
+      </c>
+      <c r="C26" t="s">
+        <v>9</v>
+      </c>
+      <c r="D26" t="s">
+        <v>16</v>
+      </c>
+      <c r="E26" t="s">
+        <v>10</v>
+      </c>
+      <c r="F26" t="s">
+        <v>16</v>
+      </c>
+      <c r="G26" t="s">
+        <v>11</v>
+      </c>
+      <c r="H26" t="s">
+        <v>16</v>
+      </c>
+      <c r="I26" t="s">
+        <v>12</v>
+      </c>
+      <c r="J26" t="s">
+        <v>16</v>
+      </c>
+      <c r="K26" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>84</v>
+      </c>
+      <c r="B27">
+        <v>0.99650000000000005</v>
+      </c>
+      <c r="C27">
+        <v>0.82138999999999995</v>
+      </c>
+      <c r="D27">
+        <v>0.76971999999999996</v>
+      </c>
+      <c r="E27">
+        <v>0.70698000000000005</v>
+      </c>
+      <c r="F27">
+        <v>0.64927999999999997</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>85</v>
+      </c>
+      <c r="B28">
+        <v>0.77380000000000004</v>
+      </c>
+      <c r="C28">
+        <v>0.99631999999999998</v>
+      </c>
+      <c r="D28">
+        <v>0.99812999999999996</v>
+      </c>
+      <c r="E28">
+        <v>0.99529000000000001</v>
+      </c>
+      <c r="F28">
+        <v>0.99839</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>86</v>
+      </c>
+      <c r="B29" t="s">
+        <v>87</v>
+      </c>
+      <c r="C29" t="s">
+        <v>88</v>
+      </c>
+      <c r="D29">
+        <v>0.95660000000000001</v>
+      </c>
+      <c r="E29">
+        <v>0.90430999999999995</v>
+      </c>
+      <c r="F29">
+        <v>0.91215000000000002</v>
+      </c>
+      <c r="G29">
+        <v>0.8639</v>
+      </c>
+      <c r="H29">
+        <v>0.96321000000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>89</v>
+      </c>
+      <c r="B30" t="s">
+        <v>87</v>
+      </c>
+      <c r="C30" t="s">
+        <v>88</v>
+      </c>
+      <c r="D30">
+        <v>0.97799999999999998</v>
+      </c>
+      <c r="E30">
+        <v>0.99246999999999996</v>
+      </c>
+      <c r="F30">
+        <v>0.99421999999999999</v>
+      </c>
+      <c r="G30">
+        <v>0.98770999999999998</v>
+      </c>
+      <c r="H30">
+        <v>0.97770000000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>90</v>
+      </c>
+      <c r="B31">
+        <v>0.83330000000000004</v>
+      </c>
+      <c r="C31">
+        <v>4.0599999999999997E-2</v>
+      </c>
+      <c r="D31">
+        <v>2.4580000000000001E-2</v>
+      </c>
+      <c r="E31">
+        <v>4.0559999999999999E-2</v>
+      </c>
+      <c r="F31">
+        <v>6.0979999999999999E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>91</v>
+      </c>
+      <c r="B32" t="s">
+        <v>76</v>
+      </c>
+      <c r="C32">
+        <v>0.83040000000000003</v>
+      </c>
+      <c r="D32">
+        <v>3.3349999999999998E-2</v>
+      </c>
+      <c r="E32">
+        <v>1.8919999999999999E-2</v>
+      </c>
+      <c r="F32">
+        <v>2.8680000000000001E-2</v>
+      </c>
+      <c r="G32">
+        <v>3.959E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>91</v>
+      </c>
+      <c r="B33" t="s">
+        <v>90</v>
+      </c>
+      <c r="C33">
+        <v>0.86809999999999998</v>
+      </c>
+      <c r="D33">
+        <v>3.6880000000000003E-2</v>
+      </c>
+      <c r="E33">
+        <v>2.0750000000000001E-2</v>
+      </c>
+      <c r="F33">
+        <v>3.3189999999999997E-2</v>
+      </c>
+      <c r="G33">
+        <v>4.1099999999999998E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>92</v>
+      </c>
+      <c r="B34" t="s">
+        <v>69</v>
+      </c>
+      <c r="C34">
+        <v>0.88519999999999999</v>
+      </c>
+      <c r="D34">
+        <v>0.90886</v>
+      </c>
+      <c r="E34">
+        <v>0.88392000000000004</v>
+      </c>
+      <c r="F34">
+        <v>0.85114000000000001</v>
+      </c>
+      <c r="G34">
+        <v>0.82384000000000002</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B36" t="s">
+        <v>84</v>
+      </c>
+      <c r="C36" t="s">
+        <v>85</v>
+      </c>
+      <c r="D36" t="s">
+        <v>86</v>
+      </c>
+      <c r="E36" t="s">
+        <v>87</v>
+      </c>
+      <c r="F36" t="s">
+        <v>88</v>
+      </c>
+      <c r="G36" t="s">
+        <v>89</v>
+      </c>
+      <c r="H36" t="s">
+        <v>87</v>
+      </c>
+      <c r="I36" t="s">
+        <v>88</v>
+      </c>
+      <c r="J36" t="s">
+        <v>14</v>
+      </c>
+      <c r="K36" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>16</v>
+      </c>
+      <c r="B37" t="s">
+        <v>9</v>
+      </c>
+      <c r="C37">
+        <v>0.9965098</v>
+      </c>
+      <c r="D37">
+        <v>0.77381089999999997</v>
+      </c>
+      <c r="E37">
+        <v>0.95655860000000004</v>
+      </c>
+      <c r="F37">
+        <v>0.97795410000000005</v>
+      </c>
+      <c r="G37">
+        <v>0.95655860000000004</v>
+      </c>
+      <c r="H37">
+        <v>0.9965098</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>16</v>
+      </c>
+      <c r="B38" t="s">
+        <v>10</v>
+      </c>
+      <c r="C38">
+        <v>0.82139450000000003</v>
+      </c>
+      <c r="D38">
+        <v>0.99632200000000004</v>
+      </c>
+      <c r="E38">
+        <v>0.90431130000000004</v>
+      </c>
+      <c r="F38">
+        <v>0.99247110000000005</v>
+      </c>
+      <c r="G38">
+        <v>0.90431130000000004</v>
+      </c>
+      <c r="H38">
+        <v>0.82139450000000003</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>16</v>
+      </c>
+      <c r="B39" t="s">
+        <v>11</v>
+      </c>
+      <c r="C39">
+        <v>0.76971610000000001</v>
+      </c>
+      <c r="D39">
+        <v>0.99813149999999995</v>
+      </c>
+      <c r="E39">
+        <v>0.91214949999999995</v>
+      </c>
+      <c r="F39">
+        <v>0.99421859999999995</v>
+      </c>
+      <c r="G39">
+        <v>0.91214949999999995</v>
+      </c>
+      <c r="H39">
+        <v>0.76971610000000001</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>16</v>
+      </c>
+      <c r="B40" t="s">
+        <v>12</v>
+      </c>
+      <c r="C40">
+        <v>0.70697900000000002</v>
+      </c>
+      <c r="D40">
+        <v>0.9952915</v>
+      </c>
+      <c r="E40">
+        <v>0.8639019</v>
+      </c>
+      <c r="F40">
+        <v>0.9877068</v>
+      </c>
+      <c r="G40">
+        <v>0.8639019</v>
+      </c>
+      <c r="H40">
+        <v>0.70697900000000002</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>16</v>
+      </c>
+      <c r="B41" t="s">
+        <v>13</v>
+      </c>
+      <c r="C41">
+        <v>0.64928459999999999</v>
+      </c>
+      <c r="D41">
+        <v>0.99838950000000004</v>
+      </c>
+      <c r="E41">
+        <v>0.96320749999999999</v>
+      </c>
+      <c r="F41">
+        <v>0.97769779999999995</v>
+      </c>
+      <c r="G41">
+        <v>0.96320749999999999</v>
+      </c>
+      <c r="H41">
+        <v>0.64928459999999999</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B42" t="s">
+        <v>17</v>
+      </c>
+      <c r="C42" t="s">
+        <v>90</v>
+      </c>
+      <c r="D42" t="s">
+        <v>91</v>
+      </c>
+      <c r="E42" t="s">
+        <v>76</v>
+      </c>
+      <c r="F42" t="s">
+        <v>91</v>
+      </c>
+      <c r="G42" t="s">
+        <v>90</v>
+      </c>
+      <c r="H42" t="s">
+        <v>92</v>
+      </c>
+      <c r="I42" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>16</v>
+      </c>
+      <c r="B43" t="s">
+        <v>9</v>
+      </c>
+      <c r="C43">
+        <v>0.97612560000000004</v>
+      </c>
+      <c r="D43">
+        <v>0.83327839999999997</v>
+      </c>
+      <c r="E43">
+        <v>0.83037013000000004</v>
+      </c>
+      <c r="F43">
+        <v>0.86808072999999997</v>
+      </c>
+      <c r="G43">
+        <v>0.88516039999999996</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>16</v>
+      </c>
+      <c r="B44" t="s">
+        <v>10</v>
+      </c>
+      <c r="C44">
+        <v>0.86086090000000004</v>
+      </c>
+      <c r="D44">
+        <v>4.0599490000000002E-2</v>
+      </c>
+      <c r="E44">
+        <v>3.3348200000000001E-2</v>
+      </c>
+      <c r="F44">
+        <v>3.6876899999999997E-2</v>
+      </c>
+      <c r="G44">
+        <v>0.90885819999999995</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>16</v>
+      </c>
+      <c r="B45" t="s">
+        <v>11</v>
+      </c>
+      <c r="C45">
+        <v>0.83490160000000002</v>
+      </c>
+      <c r="D45">
+        <v>2.4584600000000002E-2</v>
+      </c>
+      <c r="E45">
+        <v>1.8923160000000001E-2</v>
+      </c>
+      <c r="F45">
+        <v>2.0745679999999999E-2</v>
+      </c>
+      <c r="G45">
+        <v>0.88392380000000004</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>16</v>
+      </c>
+      <c r="B46" t="s">
+        <v>12</v>
+      </c>
+      <c r="C46">
+        <v>0.77760249999999997</v>
+      </c>
+      <c r="D46">
+        <v>4.0560720000000001E-2</v>
+      </c>
+      <c r="E46">
+        <v>2.8675570000000001E-2</v>
+      </c>
+      <c r="F46">
+        <v>3.3193090000000001E-2</v>
+      </c>
+      <c r="G46">
+        <v>0.85113519999999998</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>16</v>
+      </c>
+      <c r="B47" t="s">
+        <v>13</v>
+      </c>
+      <c r="C47">
+        <v>0.7756885</v>
+      </c>
+      <c r="D47">
+        <v>6.0976790000000003E-2</v>
+      </c>
+      <c r="E47">
+        <v>3.9591290000000001E-2</v>
+      </c>
+      <c r="F47">
+        <v>4.1103590000000002E-2</v>
+      </c>
+      <c r="G47">
+        <v>0.82383700000000004</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>62</v>
+      </c>
+      <c r="B49" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>64</v>
+      </c>
+      <c r="B50" t="s">
+        <v>65</v>
+      </c>
+      <c r="C50" t="s">
+        <v>66</v>
+      </c>
+      <c r="D50" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B52" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>8</v>
+      </c>
+      <c r="B53" t="s">
+        <v>9</v>
+      </c>
+      <c r="C53" t="s">
+        <v>10</v>
+      </c>
+      <c r="D53" t="s">
+        <v>11</v>
+      </c>
+      <c r="E53" t="s">
+        <v>12</v>
+      </c>
+      <c r="F53" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B54" t="s">
+        <v>9</v>
+      </c>
+      <c r="C54">
+        <v>38289</v>
+      </c>
+      <c r="D54">
+        <v>281</v>
+      </c>
+      <c r="E54">
+        <v>221</v>
+      </c>
+      <c r="F54">
+        <v>661</v>
+      </c>
+      <c r="G54">
+        <v>1510</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B55" t="s">
+        <v>10</v>
+      </c>
+      <c r="C55">
+        <v>23</v>
+      </c>
+      <c r="D55">
+        <v>1517</v>
+      </c>
+      <c r="E55">
+        <v>15</v>
+      </c>
+      <c r="F55">
+        <v>208</v>
+      </c>
+      <c r="G55">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B56" t="s">
+        <v>11</v>
+      </c>
+      <c r="C56">
+        <v>80</v>
+      </c>
+      <c r="D56">
+        <v>19</v>
+      </c>
+      <c r="E56">
+        <v>647</v>
+      </c>
+      <c r="F56">
+        <v>57</v>
+      </c>
+      <c r="G56">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B57" t="s">
+        <v>12</v>
+      </c>
+      <c r="C57">
+        <v>123</v>
+      </c>
+      <c r="D57">
+        <v>99</v>
+      </c>
+      <c r="E57">
+        <v>28</v>
+      </c>
+      <c r="F57">
+        <v>1552</v>
+      </c>
+      <c r="G57">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B58" t="s">
+        <v>13</v>
+      </c>
+      <c r="C58">
+        <v>38</v>
+      </c>
+      <c r="D58">
+        <v>9</v>
+      </c>
+      <c r="E58">
+        <v>7</v>
+      </c>
+      <c r="F58">
+        <v>18</v>
+      </c>
+      <c r="G58">
+        <v>1192</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>68</v>
+      </c>
+      <c r="B60" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B62" t="s">
+        <v>69</v>
+      </c>
+      <c r="C62" t="s">
+        <v>70</v>
+      </c>
+      <c r="D62">
+        <v>0.92569999999999997</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B63" s="9">
+        <v>0.95</v>
+      </c>
+      <c r="C63" t="s">
+        <v>71</v>
+      </c>
+      <c r="D63" t="s">
+        <v>70</v>
+      </c>
+      <c r="E63" t="s">
+        <v>94</v>
+      </c>
+      <c r="F63" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B64" t="s">
+        <v>74</v>
+      </c>
+      <c r="C64" t="s">
+        <v>75</v>
+      </c>
+      <c r="D64" t="s">
+        <v>76</v>
+      </c>
+      <c r="E64" t="s">
+        <v>70</v>
+      </c>
+      <c r="F64">
+        <v>0.82620000000000005</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B65" t="s">
+        <v>77</v>
+      </c>
+      <c r="C65" t="s">
+        <v>78</v>
+      </c>
+      <c r="D65" t="s">
+        <v>21</v>
+      </c>
+      <c r="E65" t="s">
+        <v>79</v>
+      </c>
+      <c r="F65" t="s">
+        <v>70</v>
+      </c>
+      <c r="G65" t="s">
+        <v>80</v>
+      </c>
+      <c r="H65" s="10">
+        <v>2.2E-16</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B67" t="s">
+        <v>81</v>
+      </c>
+      <c r="C67" t="s">
+        <v>70</v>
+      </c>
+      <c r="D67">
+        <v>0.72389999999999999</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B68" t="s">
+        <v>82</v>
+      </c>
+      <c r="C68" t="s">
+        <v>29</v>
+      </c>
+      <c r="D68" t="s">
+        <v>77</v>
+      </c>
+      <c r="E68" t="s">
+        <v>70</v>
+      </c>
+      <c r="F68" t="s">
+        <v>80</v>
+      </c>
+      <c r="G68" s="10">
+        <v>2.2E-16</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>67</v>
+      </c>
+      <c r="B70" t="s">
+        <v>83</v>
+      </c>
+      <c r="C70" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B72" t="s">
+        <v>16</v>
+      </c>
+      <c r="C72" t="s">
+        <v>9</v>
+      </c>
+      <c r="D72" t="s">
+        <v>16</v>
+      </c>
+      <c r="E72" t="s">
+        <v>10</v>
+      </c>
+      <c r="F72" t="s">
+        <v>16</v>
+      </c>
+      <c r="G72" t="s">
+        <v>11</v>
+      </c>
+      <c r="H72" t="s">
+        <v>16</v>
+      </c>
+      <c r="I72" t="s">
+        <v>12</v>
+      </c>
+      <c r="J72" t="s">
+        <v>16</v>
+      </c>
+      <c r="K72" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>84</v>
+      </c>
+      <c r="B73">
+        <v>0.99319999999999997</v>
+      </c>
+      <c r="C73">
+        <v>0.78805000000000003</v>
+      </c>
+      <c r="D73">
+        <v>0.70479000000000003</v>
+      </c>
+      <c r="E73">
+        <v>0.62178999999999995</v>
+      </c>
+      <c r="F73">
+        <v>0.42986000000000002</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>85</v>
+      </c>
+      <c r="B74">
+        <v>0.67049999999999998</v>
+      </c>
+      <c r="C74">
+        <v>0.99390000000000001</v>
+      </c>
+      <c r="D74">
+        <v>0.99636999999999998</v>
+      </c>
+      <c r="E74">
+        <v>0.99356999999999995</v>
+      </c>
+      <c r="F74">
+        <v>0.99836000000000003</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>86</v>
+      </c>
+      <c r="B75" t="s">
+        <v>87</v>
+      </c>
+      <c r="C75" t="s">
+        <v>88</v>
+      </c>
+      <c r="D75">
+        <v>0.93469999999999998</v>
+      </c>
+      <c r="E75">
+        <v>0.84748999999999997</v>
+      </c>
+      <c r="F75">
+        <v>0.79581999999999997</v>
+      </c>
+      <c r="G75">
+        <v>0.84531999999999996</v>
+      </c>
+      <c r="H75">
+        <v>0.94303999999999999</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>89</v>
+      </c>
+      <c r="B76" t="s">
+        <v>87</v>
+      </c>
+      <c r="C76" t="s">
+        <v>88</v>
+      </c>
+      <c r="D76">
+        <v>0.95369999999999999</v>
+      </c>
+      <c r="E76">
+        <v>0.99090999999999996</v>
+      </c>
+      <c r="F76">
+        <v>0.99409000000000003</v>
+      </c>
+      <c r="G76">
+        <v>0.97894000000000003</v>
+      </c>
+      <c r="H76">
+        <v>0.96518000000000004</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>90</v>
+      </c>
+      <c r="B77">
+        <v>0.82620000000000005</v>
+      </c>
+      <c r="C77">
+        <v>4.1250000000000002E-2</v>
+      </c>
+      <c r="D77">
+        <v>1.967E-2</v>
+      </c>
+      <c r="E77">
+        <v>5.3490000000000003E-2</v>
+      </c>
+      <c r="F77">
+        <v>5.9420000000000001E-2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>91</v>
+      </c>
+      <c r="B78" t="s">
+        <v>76</v>
+      </c>
+      <c r="C78">
+        <v>0.82050000000000001</v>
+      </c>
+      <c r="D78">
+        <v>3.2509999999999997E-2</v>
+      </c>
+      <c r="E78">
+        <v>1.3860000000000001E-2</v>
+      </c>
+      <c r="F78">
+        <v>3.3259999999999998E-2</v>
+      </c>
+      <c r="G78">
+        <v>2.554E-2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>91</v>
+      </c>
+      <c r="B79" t="s">
+        <v>90</v>
+      </c>
+      <c r="C79">
+        <v>0.87780000000000002</v>
+      </c>
+      <c r="D79">
+        <v>3.8359999999999998E-2</v>
+      </c>
+      <c r="E79">
+        <v>1.7420000000000001E-2</v>
+      </c>
+      <c r="F79">
+        <v>3.934E-2</v>
+      </c>
+      <c r="G79">
+        <v>2.7089999999999999E-2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>92</v>
+      </c>
+      <c r="B80" t="s">
+        <v>69</v>
+      </c>
+      <c r="C80">
+        <v>0.83179999999999998</v>
+      </c>
+      <c r="D80">
+        <v>0.89097999999999999</v>
+      </c>
+      <c r="E80">
+        <v>0.85058</v>
+      </c>
+      <c r="F80">
+        <v>0.80767999999999995</v>
+      </c>
+      <c r="G80">
+        <v>0.71411000000000002</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B82" t="s">
+        <v>84</v>
+      </c>
+      <c r="C82" t="s">
+        <v>85</v>
+      </c>
+      <c r="D82" t="s">
+        <v>86</v>
+      </c>
+      <c r="E82" t="s">
+        <v>87</v>
+      </c>
+      <c r="F82" t="s">
+        <v>88</v>
+      </c>
+      <c r="G82" t="s">
+        <v>89</v>
+      </c>
+      <c r="H82" t="s">
+        <v>87</v>
+      </c>
+      <c r="I82" t="s">
+        <v>88</v>
+      </c>
+      <c r="J82" t="s">
+        <v>14</v>
+      </c>
+      <c r="K82" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>16</v>
+      </c>
+      <c r="B83" t="s">
+        <v>9</v>
+      </c>
+      <c r="C83">
+        <v>0.99315229999999999</v>
+      </c>
+      <c r="D83">
+        <v>0.67048819999999998</v>
+      </c>
+      <c r="E83">
+        <v>0.93474440000000003</v>
+      </c>
+      <c r="F83">
+        <v>0.95370860000000002</v>
+      </c>
+      <c r="G83">
+        <v>0.93474440000000003</v>
+      </c>
+      <c r="H83">
+        <v>0.99315229999999999</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>16</v>
+      </c>
+      <c r="B84" t="s">
+        <v>10</v>
+      </c>
+      <c r="C84">
+        <v>0.78805190000000003</v>
+      </c>
+      <c r="D84">
+        <v>0.99389810000000001</v>
+      </c>
+      <c r="E84">
+        <v>0.84748599999999996</v>
+      </c>
+      <c r="F84">
+        <v>0.99090809999999996</v>
+      </c>
+      <c r="G84">
+        <v>0.84748599999999996</v>
+      </c>
+      <c r="H84">
+        <v>0.78805190000000003</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>16</v>
+      </c>
+      <c r="B85" t="s">
+        <v>11</v>
+      </c>
+      <c r="C85">
+        <v>0.704793</v>
+      </c>
+      <c r="D85">
+        <v>0.99637129999999996</v>
+      </c>
+      <c r="E85">
+        <v>0.79581800000000003</v>
+      </c>
+      <c r="F85">
+        <v>0.99408969999999997</v>
+      </c>
+      <c r="G85">
+        <v>0.79581800000000003</v>
+      </c>
+      <c r="H85">
+        <v>0.704793</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>16</v>
+      </c>
+      <c r="B86" t="s">
+        <v>12</v>
+      </c>
+      <c r="C86">
+        <v>0.62179490000000004</v>
+      </c>
+      <c r="D86">
+        <v>0.99357019999999996</v>
+      </c>
+      <c r="E86">
+        <v>0.84531590000000001</v>
+      </c>
+      <c r="F86">
+        <v>0.97894219999999998</v>
+      </c>
+      <c r="G86">
+        <v>0.84531590000000001</v>
+      </c>
+      <c r="H86">
+        <v>0.62179490000000004</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>16</v>
+      </c>
+      <c r="B87" t="s">
+        <v>13</v>
+      </c>
+      <c r="C87">
+        <v>0.4298594</v>
+      </c>
+      <c r="D87">
+        <v>0.99835960000000001</v>
+      </c>
+      <c r="E87">
+        <v>0.94303800000000004</v>
+      </c>
+      <c r="F87">
+        <v>0.96517699999999995</v>
+      </c>
+      <c r="G87">
+        <v>0.94303800000000004</v>
+      </c>
+      <c r="H87">
+        <v>0.4298594</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B88" t="s">
+        <v>17</v>
+      </c>
+      <c r="C88" t="s">
+        <v>90</v>
+      </c>
+      <c r="D88" t="s">
+        <v>91</v>
+      </c>
+      <c r="E88" t="s">
+        <v>76</v>
+      </c>
+      <c r="F88" t="s">
+        <v>91</v>
+      </c>
+      <c r="G88" t="s">
+        <v>90</v>
+      </c>
+      <c r="H88" t="s">
+        <v>92</v>
+      </c>
+      <c r="I88" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>16</v>
+      </c>
+      <c r="B89" t="s">
+        <v>9</v>
+      </c>
+      <c r="C89">
+        <v>0.96306360000000002</v>
+      </c>
+      <c r="D89">
+        <v>0.82616522000000003</v>
+      </c>
+      <c r="E89">
+        <v>0.82050787999999997</v>
+      </c>
+      <c r="F89">
+        <v>0.87778849000000003</v>
+      </c>
+      <c r="G89">
+        <v>0.83182020000000001</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>16</v>
+      </c>
+      <c r="B90" t="s">
+        <v>10</v>
+      </c>
+      <c r="C90">
+        <v>0.81668909999999995</v>
+      </c>
+      <c r="D90">
+        <v>4.1251469999999998E-2</v>
+      </c>
+      <c r="E90">
+        <v>3.2508299999999997E-2</v>
+      </c>
+      <c r="F90">
+        <v>3.8358509999999998E-2</v>
+      </c>
+      <c r="G90">
+        <v>0.89097499999999996</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>16</v>
+      </c>
+      <c r="B91" t="s">
+        <v>11</v>
+      </c>
+      <c r="C91">
+        <v>0.74754480000000001</v>
+      </c>
+      <c r="D91">
+        <v>1.9672129999999999E-2</v>
+      </c>
+      <c r="E91">
+        <v>1.386478E-2</v>
+      </c>
+      <c r="F91">
+        <v>1.7422050000000001E-2</v>
+      </c>
+      <c r="G91">
+        <v>0.85058219999999995</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>16</v>
+      </c>
+      <c r="B92" t="s">
+        <v>12</v>
+      </c>
+      <c r="C92">
+        <v>0.71652819999999995</v>
+      </c>
+      <c r="D92">
+        <v>5.348762E-2</v>
+      </c>
+      <c r="E92">
+        <v>3.3258330000000003E-2</v>
+      </c>
+      <c r="F92">
+        <v>3.9344259999999999E-2</v>
+      </c>
+      <c r="G92">
+        <v>0.80768249999999997</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>16</v>
+      </c>
+      <c r="B93" t="s">
+        <v>13</v>
+      </c>
+      <c r="C93">
+        <v>0.59053750000000005</v>
+      </c>
+      <c r="D93">
+        <v>5.9423549999999999E-2</v>
+      </c>
+      <c r="E93">
+        <v>2.554377E-2</v>
+      </c>
+      <c r="F93">
+        <v>2.7086679999999998E-2</v>
+      </c>
+      <c r="G93">
+        <v>0.71410949999999995</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>62</v>
+      </c>
+      <c r="B95" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>64</v>
+      </c>
+      <c r="B96" t="s">
+        <v>65</v>
+      </c>
+      <c r="C96" t="s">
+        <v>66</v>
+      </c>
+      <c r="D96" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B98" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>8</v>
+      </c>
+      <c r="B99" t="s">
+        <v>9</v>
+      </c>
+      <c r="C99" t="s">
+        <v>10</v>
+      </c>
+      <c r="D99" t="s">
+        <v>11</v>
+      </c>
+      <c r="E99" t="s">
+        <v>12</v>
+      </c>
+      <c r="F99" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B100" t="s">
+        <v>9</v>
+      </c>
+      <c r="C100">
+        <v>29</v>
+      </c>
+      <c r="D100">
+        <v>0</v>
+      </c>
+      <c r="E100">
+        <v>0</v>
+      </c>
+      <c r="F100">
+        <v>0</v>
+      </c>
+      <c r="G100">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B101" t="s">
+        <v>10</v>
+      </c>
+      <c r="C101">
+        <v>0</v>
+      </c>
+      <c r="D101">
+        <v>0</v>
+      </c>
+      <c r="E101">
+        <v>0</v>
+      </c>
+      <c r="F101">
+        <v>0</v>
+      </c>
+      <c r="G101">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B102" t="s">
+        <v>11</v>
+      </c>
+      <c r="C102">
+        <v>0</v>
+      </c>
+      <c r="D102">
+        <v>0</v>
+      </c>
+      <c r="E102">
+        <v>1</v>
+      </c>
+      <c r="F102">
+        <v>0</v>
+      </c>
+      <c r="G102">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B103" t="s">
+        <v>12</v>
+      </c>
+      <c r="C103">
+        <v>0</v>
+      </c>
+      <c r="D103">
+        <v>0</v>
+      </c>
+      <c r="E103">
+        <v>0</v>
+      </c>
+      <c r="F103">
+        <v>2</v>
+      </c>
+      <c r="G103">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B104" t="s">
+        <v>13</v>
+      </c>
+      <c r="C104">
+        <v>0</v>
+      </c>
+      <c r="D104">
+        <v>0</v>
+      </c>
+      <c r="E104">
+        <v>0</v>
+      </c>
+      <c r="F104">
+        <v>0</v>
+      </c>
+      <c r="G104">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
+        <v>68</v>
+      </c>
+      <c r="B106" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B108" t="s">
+        <v>69</v>
+      </c>
+      <c r="C108" t="s">
+        <v>70</v>
+      </c>
+      <c r="D108">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B109" s="9">
+        <v>0.95</v>
+      </c>
+      <c r="C109" t="s">
+        <v>71</v>
+      </c>
+      <c r="D109" t="s">
+        <v>70</v>
+      </c>
+      <c r="E109" t="s">
+        <v>97</v>
+      </c>
+      <c r="F109" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B110" t="s">
+        <v>74</v>
+      </c>
+      <c r="C110" t="s">
+        <v>75</v>
+      </c>
+      <c r="D110" t="s">
+        <v>76</v>
+      </c>
+      <c r="E110" t="s">
+        <v>70</v>
+      </c>
+      <c r="F110">
+        <v>0.85289999999999999</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B111" t="s">
+        <v>77</v>
+      </c>
+      <c r="C111" t="s">
+        <v>78</v>
+      </c>
+      <c r="D111" t="s">
+        <v>21</v>
+      </c>
+      <c r="E111" t="s">
+        <v>79</v>
+      </c>
+      <c r="F111" t="s">
+        <v>70</v>
+      </c>
+      <c r="G111">
+        <v>4.4799999999999996E-3</v>
+      </c>
+    </row>
+    <row r="113" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B113" t="s">
+        <v>81</v>
+      </c>
+      <c r="C113" t="s">
+        <v>70</v>
+      </c>
+      <c r="D113">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B114" t="s">
+        <v>82</v>
+      </c>
+      <c r="C114" t="s">
+        <v>29</v>
+      </c>
+      <c r="D114" t="s">
+        <v>77</v>
+      </c>
+      <c r="E114" t="s">
+        <v>70</v>
+      </c>
+      <c r="F114" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="116" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A116" t="s">
+        <v>67</v>
+      </c>
+      <c r="B116" t="s">
+        <v>83</v>
+      </c>
+      <c r="C116" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="118" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B118" t="s">
+        <v>16</v>
+      </c>
+      <c r="C118" t="s">
+        <v>9</v>
+      </c>
+      <c r="D118" t="s">
+        <v>16</v>
+      </c>
+      <c r="E118" t="s">
+        <v>10</v>
+      </c>
+      <c r="F118" t="s">
+        <v>16</v>
+      </c>
+      <c r="G118" t="s">
+        <v>11</v>
+      </c>
+      <c r="H118" t="s">
+        <v>16</v>
+      </c>
+      <c r="I118" t="s">
+        <v>12</v>
+      </c>
+      <c r="J118" t="s">
+        <v>16</v>
+      </c>
+      <c r="K118" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="119" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A119" t="s">
+        <v>84</v>
+      </c>
+      <c r="B119">
+        <v>1</v>
+      </c>
+      <c r="C119" t="s">
+        <v>18</v>
+      </c>
+      <c r="D119">
+        <v>1</v>
+      </c>
+      <c r="E119">
+        <v>1</v>
+      </c>
+      <c r="F119">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A120" t="s">
+        <v>85</v>
+      </c>
+      <c r="B120">
+        <v>1</v>
+      </c>
+      <c r="C120">
+        <v>1</v>
+      </c>
+      <c r="D120">
+        <v>1</v>
+      </c>
+      <c r="E120">
+        <v>1</v>
+      </c>
+      <c r="F120">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A121" t="s">
+        <v>86</v>
+      </c>
+      <c r="B121" t="s">
+        <v>87</v>
+      </c>
+      <c r="C121" t="s">
+        <v>88</v>
+      </c>
+      <c r="D121">
+        <v>1</v>
+      </c>
+      <c r="E121" t="s">
+        <v>18</v>
+      </c>
+      <c r="F121">
+        <v>1</v>
+      </c>
+      <c r="G121">
+        <v>1</v>
+      </c>
+      <c r="H121">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A122" t="s">
+        <v>89</v>
+      </c>
+      <c r="B122" t="s">
+        <v>87</v>
+      </c>
+      <c r="C122" t="s">
+        <v>88</v>
+      </c>
+      <c r="D122">
+        <v>1</v>
+      </c>
+      <c r="E122" t="s">
+        <v>18</v>
+      </c>
+      <c r="F122">
+        <v>1</v>
+      </c>
+      <c r="G122">
+        <v>1</v>
+      </c>
+      <c r="H122">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A123" t="s">
+        <v>90</v>
+      </c>
+      <c r="B123">
+        <v>0.85289999999999999</v>
+      </c>
+      <c r="C123">
+        <v>0</v>
+      </c>
+      <c r="D123">
+        <v>2.9409999999999999E-2</v>
+      </c>
+      <c r="E123">
+        <v>5.8819999999999997E-2</v>
+      </c>
+      <c r="F123">
+        <v>5.8819999999999997E-2</v>
+      </c>
+    </row>
+    <row r="124" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A124" t="s">
+        <v>91</v>
+      </c>
+      <c r="B124" t="s">
+        <v>76</v>
+      </c>
+      <c r="C124">
+        <v>0.85289999999999999</v>
+      </c>
+      <c r="D124">
+        <v>0</v>
+      </c>
+      <c r="E124">
+        <v>2.9409999999999999E-2</v>
+      </c>
+      <c r="F124">
+        <v>5.8819999999999997E-2</v>
+      </c>
+      <c r="G124">
+        <v>5.8819999999999997E-2</v>
+      </c>
+    </row>
+    <row r="125" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A125" t="s">
+        <v>91</v>
+      </c>
+      <c r="B125" t="s">
+        <v>90</v>
+      </c>
+      <c r="C125">
+        <v>0.85289999999999999</v>
+      </c>
+      <c r="D125">
+        <v>0</v>
+      </c>
+      <c r="E125">
+        <v>2.9409999999999999E-2</v>
+      </c>
+      <c r="F125">
+        <v>5.8819999999999997E-2</v>
+      </c>
+      <c r="G125">
+        <v>5.8819999999999997E-2</v>
+      </c>
+    </row>
+    <row r="126" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A126" t="s">
+        <v>92</v>
+      </c>
+      <c r="B126" t="s">
+        <v>69</v>
+      </c>
+      <c r="C126">
+        <v>1</v>
+      </c>
+      <c r="D126" t="s">
+        <v>18</v>
+      </c>
+      <c r="E126">
+        <v>1</v>
+      </c>
+      <c r="F126">
+        <v>1</v>
+      </c>
+      <c r="G126">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A127" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="128" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B128" t="s">
+        <v>84</v>
+      </c>
+      <c r="C128" t="s">
+        <v>85</v>
+      </c>
+      <c r="D128" t="s">
+        <v>86</v>
+      </c>
+      <c r="E128" t="s">
+        <v>87</v>
+      </c>
+      <c r="F128" t="s">
+        <v>88</v>
+      </c>
+      <c r="G128" t="s">
+        <v>89</v>
+      </c>
+      <c r="H128" t="s">
+        <v>87</v>
+      </c>
+      <c r="I128" t="s">
+        <v>88</v>
+      </c>
+      <c r="J128" t="s">
+        <v>14</v>
+      </c>
+      <c r="K128" t="s">
+        <v>15</v>
+      </c>
+      <c r="L128" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="129" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A129" t="s">
+        <v>16</v>
+      </c>
+      <c r="B129" t="s">
+        <v>9</v>
+      </c>
+      <c r="C129">
+        <v>1</v>
+      </c>
+      <c r="D129">
+        <v>1</v>
+      </c>
+      <c r="E129">
+        <v>1</v>
+      </c>
+      <c r="F129">
+        <v>1</v>
+      </c>
+      <c r="G129">
+        <v>1</v>
+      </c>
+      <c r="H129">
+        <v>1</v>
+      </c>
+      <c r="I129">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A130" t="s">
+        <v>16</v>
+      </c>
+      <c r="B130" t="s">
+        <v>10</v>
+      </c>
+      <c r="C130" t="s">
+        <v>18</v>
+      </c>
+      <c r="D130">
+        <v>1</v>
+      </c>
+      <c r="E130" t="s">
+        <v>18</v>
+      </c>
+      <c r="F130" t="s">
+        <v>18</v>
+      </c>
+      <c r="G130" t="s">
+        <v>18</v>
+      </c>
+      <c r="H130" t="s">
+        <v>18</v>
+      </c>
+      <c r="I130" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="131" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A131" t="s">
+        <v>16</v>
+      </c>
+      <c r="B131" t="s">
+        <v>11</v>
+      </c>
+      <c r="C131">
+        <v>1</v>
+      </c>
+      <c r="D131">
+        <v>1</v>
+      </c>
+      <c r="E131">
+        <v>1</v>
+      </c>
+      <c r="F131">
+        <v>1</v>
+      </c>
+      <c r="G131">
+        <v>1</v>
+      </c>
+      <c r="H131">
+        <v>1</v>
+      </c>
+      <c r="I131">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="132" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A132" t="s">
+        <v>16</v>
+      </c>
+      <c r="B132" t="s">
+        <v>12</v>
+      </c>
+      <c r="C132">
+        <v>1</v>
+      </c>
+      <c r="D132">
+        <v>1</v>
+      </c>
+      <c r="E132">
+        <v>1</v>
+      </c>
+      <c r="F132">
+        <v>1</v>
+      </c>
+      <c r="G132">
+        <v>1</v>
+      </c>
+      <c r="H132">
+        <v>1</v>
+      </c>
+      <c r="I132">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A133" t="s">
+        <v>16</v>
+      </c>
+      <c r="B133" t="s">
+        <v>13</v>
+      </c>
+      <c r="C133">
+        <v>1</v>
+      </c>
+      <c r="D133">
+        <v>1</v>
+      </c>
+      <c r="E133">
+        <v>1</v>
+      </c>
+      <c r="F133">
+        <v>1</v>
+      </c>
+      <c r="G133">
+        <v>1</v>
+      </c>
+      <c r="H133">
+        <v>1</v>
+      </c>
+      <c r="I133">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="134" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B134" t="s">
+        <v>90</v>
+      </c>
+      <c r="C134" t="s">
+        <v>91</v>
+      </c>
+      <c r="D134" t="s">
+        <v>76</v>
+      </c>
+      <c r="E134" t="s">
+        <v>91</v>
+      </c>
+      <c r="F134" t="s">
+        <v>90</v>
+      </c>
+      <c r="G134" t="s">
+        <v>92</v>
+      </c>
+      <c r="H134" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="135" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A135" t="s">
+        <v>16</v>
+      </c>
+      <c r="B135" t="s">
+        <v>9</v>
+      </c>
+      <c r="C135">
+        <v>0.85294117999999997</v>
+      </c>
+      <c r="D135">
+        <v>0.85294117999999997</v>
+      </c>
+      <c r="E135">
+        <v>0.85294117999999997</v>
+      </c>
+      <c r="F135">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A136" t="s">
+        <v>16</v>
+      </c>
+      <c r="B136" t="s">
+        <v>10</v>
+      </c>
+      <c r="C136">
+        <v>0</v>
+      </c>
+      <c r="D136">
+        <v>0</v>
+      </c>
+      <c r="E136">
+        <v>0</v>
+      </c>
+      <c r="F136" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="137" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A137" t="s">
+        <v>16</v>
+      </c>
+      <c r="B137" t="s">
+        <v>11</v>
+      </c>
+      <c r="C137">
+        <v>2.9411759999999999E-2</v>
+      </c>
+      <c r="D137">
+        <v>2.9411759999999999E-2</v>
+      </c>
+      <c r="E137">
+        <v>2.9411759999999999E-2</v>
+      </c>
+      <c r="F137">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="138" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A138" t="s">
+        <v>16</v>
+      </c>
+      <c r="B138" t="s">
+        <v>12</v>
+      </c>
+      <c r="C138">
+        <v>5.8823529999999999E-2</v>
+      </c>
+      <c r="D138">
+        <v>5.8823529999999999E-2</v>
+      </c>
+      <c r="E138">
+        <v>5.8823529999999999E-2</v>
+      </c>
+      <c r="F138">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="139" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A139" t="s">
+        <v>16</v>
+      </c>
+      <c r="B139" t="s">
+        <v>13</v>
+      </c>
+      <c r="C139">
+        <v>5.8823529999999999E-2</v>
+      </c>
+      <c r="D139">
+        <v>5.8823529999999999E-2</v>
+      </c>
+      <c r="E139">
+        <v>5.8823529999999999E-2</v>
+      </c>
+      <c r="F139">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B370712F-D1E3-A142-9145-22001148789D}">
-  <dimension ref="A1:H48"/>
+  <dimension ref="A1:K48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView topLeftCell="D10" workbookViewId="0">
+      <selection activeCell="M33" sqref="M33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3772,11 +6409,11 @@
     <col min="1" max="8" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="6"/>
       <c r="B2" s="6" t="s">
         <v>41</v>
@@ -3788,7 +6425,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>0</v>
       </c>
@@ -3802,7 +6439,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>20</v>
       </c>
@@ -3816,7 +6453,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>38</v>
       </c>
@@ -3830,7 +6467,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>37</v>
       </c>
@@ -3844,19 +6481,52 @@
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="B10" s="16"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="17" t="s">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="3">
+        <v>204566</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="30"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E10" s="31"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="H10" s="26"/>
+      <c r="I10" s="26"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="3"/>
       <c r="B11" s="3" t="s">
         <v>47</v>
@@ -3871,8 +6541,15 @@
       <c r="F11" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G11" s="1"/>
+      <c r="H11" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>4</v>
       </c>
@@ -3891,8 +6568,17 @@
       <c r="F12" s="1">
         <v>0.92360940000000002</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G12" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I12" s="1">
+        <v>0.95099999999999996</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>5</v>
       </c>
@@ -3911,8 +6597,17 @@
       <c r="F13" s="1">
         <v>0.91361829999999999</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G13" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I13" s="1">
+        <v>0.92600000000000005</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>6</v>
       </c>
@@ -3931,20 +6626,34 @@
       <c r="F14" s="1">
         <v>0.93055560000000004</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="16" t="s">
+      <c r="G14" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I14" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="16"/>
-      <c r="C15" s="16"/>
-      <c r="D15" s="17" t="s">
+      <c r="B15" s="30"/>
+      <c r="C15" s="30"/>
+      <c r="D15" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="E15" s="17"/>
-      <c r="F15" s="17"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E15" s="31"/>
+      <c r="F15" s="31"/>
+      <c r="G15" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="H15" s="26"/>
+      <c r="I15" s="26"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="3"/>
       <c r="B16" s="3" t="s">
         <v>47</v>
@@ -3959,8 +6668,15 @@
       <c r="F16" s="3" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G16" s="3"/>
+      <c r="H16" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>29</v>
       </c>
@@ -3979,701 +6695,973 @@
       <c r="F17" s="1">
         <v>0.22448979999999999</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C21" s="16" t="s">
+      <c r="G17" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+      <c r="A20" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="B20" s="27"/>
+      <c r="C20" s="27"/>
+      <c r="D20" s="27"/>
+      <c r="E20" s="27"/>
+      <c r="F20" s="27"/>
+      <c r="G20" s="27"/>
+      <c r="H20" s="27"/>
+      <c r="I20" s="27"/>
+      <c r="J20" s="27"/>
+      <c r="K20" s="27"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A21" s="15"/>
+      <c r="B21" s="15"/>
+      <c r="C21" s="32" t="s">
+        <v>103</v>
+      </c>
+      <c r="D21" s="32"/>
+      <c r="E21" s="32"/>
+      <c r="F21" s="33" t="s">
         <v>49</v>
       </c>
-      <c r="D21" s="16"/>
-      <c r="E21" s="16"/>
-      <c r="F21" s="17" t="s">
-        <v>49</v>
-      </c>
-      <c r="G21" s="17"/>
-      <c r="H21" s="17"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A22" s="15" t="s">
+      <c r="G21" s="33"/>
+      <c r="H21" s="33"/>
+      <c r="I21" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="J21" s="25"/>
+      <c r="K21" s="25"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A22" s="29" t="s">
         <v>50</v>
       </c>
-      <c r="B22" s="15"/>
-      <c r="C22" s="11"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="12"/>
-      <c r="G22" s="12"/>
-      <c r="H22" s="12"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A23" s="7" t="s">
+      <c r="B22" s="29"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="16"/>
+      <c r="F22" s="17"/>
+      <c r="G22" s="17"/>
+      <c r="H22" s="17"/>
+      <c r="I22" s="17"/>
+      <c r="J22" s="17"/>
+      <c r="K22" s="17"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A23" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="B23" s="7"/>
-      <c r="C23" s="13" t="s">
+      <c r="B23" s="18"/>
+      <c r="C23" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="D23" s="13" t="s">
+      <c r="D23" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="E23" s="11" t="s">
+      <c r="E23" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="F23" s="11" t="s">
+      <c r="F23" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="G23" s="11" t="s">
+      <c r="G23" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="H23" s="11" t="s">
+      <c r="H23" s="16" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A24" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B24" s="7" t="s">
+      <c r="I23" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="J23" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="K23" s="16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A24" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B24" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="C24" s="11">
+      <c r="C24" s="16">
         <v>0.92919289999999999</v>
       </c>
-      <c r="D24" s="11">
+      <c r="D24" s="16">
         <v>0.98655126000000004</v>
       </c>
-      <c r="E24" s="11">
+      <c r="E24" s="16">
         <v>0.95701340000000001</v>
       </c>
-      <c r="F24" s="11">
+      <c r="F24" s="16">
         <v>0.97651509999999997</v>
       </c>
-      <c r="G24" s="11">
+      <c r="G24" s="16">
         <v>0.98489930000000003</v>
       </c>
-      <c r="H24" s="11">
+      <c r="H24" s="16">
         <v>0.98068929999999999</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A25" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B25" s="7" t="s">
+      <c r="I24" s="16">
+        <v>0.95655860000000004</v>
+      </c>
+      <c r="J24" s="16">
+        <v>0.9965098</v>
+      </c>
+      <c r="K24" s="16">
+        <v>0.97612560000000004</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A25" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B25" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="C25" s="11">
+      <c r="C25" s="16">
         <v>0.63087669999999996</v>
       </c>
-      <c r="D25" s="11">
+      <c r="D25" s="16">
         <v>0.47421203000000001</v>
       </c>
-      <c r="E25" s="11">
+      <c r="E25" s="16">
         <v>0.54143949999999996</v>
       </c>
-      <c r="F25" s="11">
+      <c r="F25" s="16">
         <v>0.67963050000000003</v>
       </c>
-      <c r="G25" s="11">
+      <c r="G25" s="16">
         <v>0.66762180000000004</v>
       </c>
-      <c r="H25" s="11">
+      <c r="H25" s="16">
         <v>0.67357259999999997</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A26" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B26" s="7" t="s">
+      <c r="I25" s="16">
+        <v>0.90431130000000004</v>
+      </c>
+      <c r="J25" s="16">
+        <v>0.82139450000000003</v>
+      </c>
+      <c r="K25" s="16">
+        <v>0.86086090000000004</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A26" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B26" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="C26" s="11">
+      <c r="C26" s="16">
         <v>0.67515919999999996</v>
       </c>
-      <c r="D26" s="11">
+      <c r="D26" s="16">
         <v>8.3596210000000004E-2</v>
       </c>
-      <c r="E26" s="11">
+      <c r="E26" s="16">
         <v>0.14877190000000001</v>
       </c>
-      <c r="F26" s="11">
+      <c r="F26" s="16">
         <v>0.88604649999999996</v>
       </c>
-      <c r="G26" s="11">
+      <c r="G26" s="16">
         <v>0.3004732</v>
       </c>
-      <c r="H26" s="11">
+      <c r="H26" s="16">
         <v>0.44876329999999998</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A27" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B27" s="7" t="s">
+      <c r="I26" s="16">
+        <v>0.91214949999999995</v>
+      </c>
+      <c r="J26" s="16">
+        <v>0.76971610000000001</v>
+      </c>
+      <c r="K26" s="16">
+        <v>0.83490160000000002</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A27" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B27" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="C27" s="11">
+      <c r="C27" s="16">
         <v>0.59290779999999998</v>
       </c>
-      <c r="D27" s="11">
+      <c r="D27" s="16">
         <v>0.39961759000000002</v>
       </c>
-      <c r="E27" s="11">
+      <c r="E27" s="16">
         <v>0.47744150000000002</v>
       </c>
-      <c r="F27" s="11">
+      <c r="F27" s="16">
         <v>0.47021810000000003</v>
       </c>
-      <c r="G27" s="11">
+      <c r="G27" s="16">
         <v>0.53585090000000002</v>
       </c>
-      <c r="H27" s="11">
+      <c r="H27" s="16">
         <v>0.5008937</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A28" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B28" s="7" t="s">
+      <c r="I27" s="16">
+        <v>0.8639019</v>
+      </c>
+      <c r="J27" s="16">
+        <v>0.70697900000000002</v>
+      </c>
+      <c r="K27" s="16">
+        <v>0.77760249999999997</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A28" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B28" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="C28" s="11">
+      <c r="C28" s="16">
         <v>0.79572189999999998</v>
       </c>
-      <c r="D28" s="11">
+      <c r="D28" s="16">
         <v>0.70969793000000003</v>
       </c>
-      <c r="E28" s="11">
+      <c r="E28" s="16">
         <v>0.75025209999999998</v>
       </c>
-      <c r="F28" s="11">
+      <c r="F28" s="16">
         <v>0.71687999999999996</v>
       </c>
-      <c r="G28" s="11">
+      <c r="G28" s="16">
         <v>0.7656598</v>
       </c>
-      <c r="H28" s="11">
+      <c r="H28" s="16">
         <v>0.7404674</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A29" s="7" t="s">
+      <c r="I28" s="16">
+        <v>0.96320749999999999</v>
+      </c>
+      <c r="J28" s="16">
+        <v>0.64928459999999999</v>
+      </c>
+      <c r="K28" s="16">
+        <v>0.7756885</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A29" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="B29" s="7"/>
-      <c r="C29" s="11" t="s">
+      <c r="B29" s="18"/>
+      <c r="C29" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="D29" s="11" t="s">
+      <c r="D29" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="E29" s="11" t="s">
+      <c r="E29" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="F29" s="11" t="s">
+      <c r="F29" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="G29" s="11" t="s">
+      <c r="G29" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="H29" s="11" t="s">
+      <c r="H29" s="16" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A30" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B30" s="7" t="s">
+      <c r="I29" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="J29" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="K29" s="16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A30" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B30" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="C30" s="11">
+      <c r="C30" s="16">
         <v>0.93545920000000005</v>
       </c>
-      <c r="D30" s="11">
+      <c r="D30" s="16">
         <v>0.98236193999999999</v>
       </c>
-      <c r="E30" s="11">
+      <c r="E30" s="16">
         <v>0.95833699999999999</v>
       </c>
-      <c r="F30" s="11">
+      <c r="F30" s="16">
         <v>0.97905730000000002</v>
       </c>
-      <c r="G30" s="11">
+      <c r="G30" s="16">
         <v>0.9773558</v>
       </c>
-      <c r="H30" s="11">
+      <c r="H30" s="16">
         <v>0.97820580000000001</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A31" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B31" s="7" t="s">
+      <c r="I30" s="16">
+        <v>0.93474440000000003</v>
+      </c>
+      <c r="J30" s="16">
+        <v>0.99315229999999999</v>
+      </c>
+      <c r="K30" s="16">
+        <v>0.96306360000000002</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A31" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B31" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="C31" s="11">
+      <c r="C31" s="16">
         <v>0.61610109999999996</v>
       </c>
-      <c r="D31" s="11">
+      <c r="D31" s="16">
         <v>0.48103896000000002</v>
       </c>
-      <c r="E31" s="11">
+      <c r="E31" s="16">
         <v>0.54025670000000003</v>
       </c>
-      <c r="F31" s="11">
+      <c r="F31" s="16">
         <v>0.64760910000000005</v>
       </c>
-      <c r="G31" s="11">
+      <c r="G31" s="16">
         <v>0.64727270000000003</v>
       </c>
-      <c r="H31" s="11">
+      <c r="H31" s="16">
         <v>0.64744089999999999</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A32" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B32" s="7" t="s">
+      <c r="I31" s="16">
+        <v>0.84748599999999996</v>
+      </c>
+      <c r="J31" s="16">
+        <v>0.78805190000000003</v>
+      </c>
+      <c r="K31" s="16">
+        <v>0.81668909999999995</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A32" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B32" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="C32" s="11">
+      <c r="C32" s="16">
         <v>0.4468085</v>
       </c>
-      <c r="D32" s="11">
+      <c r="D32" s="16">
         <v>6.8627450000000007E-2</v>
       </c>
-      <c r="E32" s="11">
+      <c r="E32" s="16">
         <v>0.11898019999999999</v>
       </c>
-      <c r="F32" s="11">
+      <c r="F32" s="16">
         <v>0.86723159999999999</v>
       </c>
-      <c r="G32" s="11">
+      <c r="G32" s="16">
         <v>0.33442270000000002</v>
       </c>
-      <c r="H32" s="11">
+      <c r="H32" s="16">
         <v>0.48270439999999998</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A33" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B33" s="7" t="s">
+      <c r="I32" s="16">
+        <v>0.79581800000000003</v>
+      </c>
+      <c r="J32" s="16">
+        <v>0.704793</v>
+      </c>
+      <c r="K32" s="16">
+        <v>0.74754480000000001</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A33" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B33" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="C33" s="11">
+      <c r="C33" s="16">
         <v>0.58284179999999997</v>
       </c>
-      <c r="D33" s="11">
+      <c r="D33" s="16">
         <v>0.43549679000000002</v>
       </c>
-      <c r="E33" s="11">
+      <c r="E33" s="16">
         <v>0.49850949999999999</v>
       </c>
-      <c r="F33" s="11">
+      <c r="F33" s="16">
         <v>0.5057471</v>
       </c>
-      <c r="G33" s="11">
+      <c r="G33" s="16">
         <v>0.52884620000000004</v>
       </c>
-      <c r="H33" s="11">
+      <c r="H33" s="16">
         <v>0.51703880000000002</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A34" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B34" s="7" t="s">
+      <c r="I33" s="16">
+        <v>0.84531590000000001</v>
+      </c>
+      <c r="J33" s="16">
+        <v>0.62179490000000004</v>
+      </c>
+      <c r="K33" s="16">
+        <v>0.71652819999999995</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A34" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B34" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="C34" s="11">
+      <c r="C34" s="16">
         <v>0.73670409999999997</v>
       </c>
-      <c r="D34" s="11">
+      <c r="D34" s="16">
         <v>0.70934006000000005</v>
       </c>
-      <c r="E34" s="11">
+      <c r="E34" s="16">
         <v>0.72276320000000005</v>
       </c>
-      <c r="F34" s="11">
+      <c r="F34" s="16">
         <v>0.63233059999999996</v>
       </c>
-      <c r="G34" s="11">
+      <c r="G34" s="16">
         <v>0.75045079999999997</v>
       </c>
-      <c r="H34" s="11">
+      <c r="H34" s="16">
         <v>0.6863456</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A35" s="7" t="s">
+      <c r="I34" s="16">
+        <v>0.94303800000000004</v>
+      </c>
+      <c r="J34" s="16">
+        <v>0.4298594</v>
+      </c>
+      <c r="K34" s="16">
+        <v>0.59053750000000005</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A35" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B35" s="7"/>
-      <c r="C35" s="11" t="s">
+      <c r="B35" s="18"/>
+      <c r="C35" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="D35" s="11" t="s">
+      <c r="D35" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="E35" s="11" t="s">
+      <c r="E35" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="F35" s="11" t="s">
+      <c r="F35" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="G35" s="11" t="s">
+      <c r="G35" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="H35" s="11" t="s">
+      <c r="H35" s="16" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A36" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B36" s="7" t="s">
+      <c r="I35" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="J35" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="K35" s="16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A36" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B36" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="C36" s="11">
+      <c r="C36" s="16">
         <v>0.92424240000000002</v>
       </c>
-      <c r="D36" s="11">
-        <v>1</v>
-      </c>
-      <c r="E36" s="11">
+      <c r="D36" s="16">
+        <v>1</v>
+      </c>
+      <c r="E36" s="16">
         <v>0.96062990000000004</v>
       </c>
-      <c r="F36" s="11">
+      <c r="F36" s="16">
         <v>0.96825399999999995</v>
       </c>
-      <c r="G36" s="11">
-        <v>1</v>
-      </c>
-      <c r="H36" s="11">
+      <c r="G36" s="16">
+        <v>1</v>
+      </c>
+      <c r="H36" s="16">
         <v>0.98387100000000005</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A37" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B37" s="7" t="s">
+      <c r="I36" s="16">
+        <v>1</v>
+      </c>
+      <c r="J36" s="16">
+        <v>1</v>
+      </c>
+      <c r="K36" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A37" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B37" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="C37" s="11">
-        <v>0</v>
-      </c>
-      <c r="D37" s="11" t="s">
+      <c r="C37" s="16">
+        <v>0</v>
+      </c>
+      <c r="D37" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="E37" s="11" t="s">
+      <c r="E37" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="F37" s="11">
-        <v>0</v>
-      </c>
-      <c r="G37" s="11" t="s">
+      <c r="F37" s="16">
+        <v>0</v>
+      </c>
+      <c r="G37" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="H37" s="11" t="s">
+      <c r="H37" s="16" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A38" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B38" s="7" t="s">
+      <c r="I37" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="J37" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="K37" s="16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A38" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B38" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="C38" s="11" t="s">
+      <c r="C38" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="D38" s="11">
-        <v>0</v>
-      </c>
-      <c r="E38" s="11" t="s">
+      <c r="D38" s="16">
+        <v>0</v>
+      </c>
+      <c r="E38" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="F38" s="11">
-        <v>1</v>
-      </c>
-      <c r="G38" s="11">
+      <c r="F38" s="16">
+        <v>1</v>
+      </c>
+      <c r="G38" s="16">
         <v>0.5</v>
       </c>
-      <c r="H38" s="11">
+      <c r="H38" s="16">
         <v>0.66666669999999995</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A39" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B39" s="7" t="s">
+      <c r="I38" s="16">
+        <v>1</v>
+      </c>
+      <c r="J38" s="16">
+        <v>1</v>
+      </c>
+      <c r="K38" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A39" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B39" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="C39" s="11">
+      <c r="C39" s="16">
         <v>0.3333333</v>
       </c>
-      <c r="D39" s="11">
+      <c r="D39" s="16">
         <v>0.14285709999999999</v>
       </c>
-      <c r="E39" s="11">
+      <c r="E39" s="16">
         <v>0.2</v>
       </c>
-      <c r="F39" s="11">
+      <c r="F39" s="16">
         <v>0.75</v>
       </c>
-      <c r="G39" s="11">
+      <c r="G39" s="16">
         <v>0.42857139999999999</v>
       </c>
-      <c r="H39" s="11">
+      <c r="H39" s="16">
         <v>0.54545449999999995</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A40" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B40" s="7" t="s">
+      <c r="I39" s="16">
+        <v>1</v>
+      </c>
+      <c r="J39" s="16">
+        <v>1</v>
+      </c>
+      <c r="K39" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A40" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B40" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="C40" s="11">
-        <v>1</v>
-      </c>
-      <c r="D40" s="11">
-        <v>1</v>
-      </c>
-      <c r="E40" s="11">
-        <v>1</v>
-      </c>
-      <c r="F40" s="11">
+      <c r="C40" s="16">
+        <v>1</v>
+      </c>
+      <c r="D40" s="16">
+        <v>1</v>
+      </c>
+      <c r="E40" s="16">
+        <v>1</v>
+      </c>
+      <c r="F40" s="16">
         <v>0.66666669999999995</v>
       </c>
-      <c r="G40" s="11">
-        <v>1</v>
-      </c>
-      <c r="H40" s="11">
+      <c r="G40" s="16">
+        <v>1</v>
+      </c>
+      <c r="H40" s="16">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A41" s="14" t="s">
+      <c r="I40" s="16">
+        <v>1</v>
+      </c>
+      <c r="J40" s="16">
+        <v>1</v>
+      </c>
+      <c r="K40" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A41" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="B41" s="14"/>
-      <c r="C41" s="9" t="s">
+      <c r="B41" s="28"/>
+      <c r="C41" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="D41" s="9" t="s">
+      <c r="D41" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="E41" s="9" t="s">
+      <c r="E41" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="F41" s="9" t="s">
+      <c r="F41" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="G41" s="9" t="s">
+      <c r="G41" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="H41" s="9" t="s">
+      <c r="H41" s="19" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A42" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B42" s="8" t="s">
+      <c r="I41" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="J41" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="K41" s="19" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A42" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="B42" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="C42" s="10" t="s">
+      <c r="C42" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="D42" s="10">
-        <v>0</v>
-      </c>
-      <c r="E42" s="10" t="s">
+      <c r="D42" s="21">
+        <v>0</v>
+      </c>
+      <c r="E42" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="F42" s="10" t="s">
+      <c r="F42" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="G42" s="10">
-        <v>0</v>
-      </c>
-      <c r="H42" s="10" t="s">
+      <c r="G42" s="21">
+        <v>0</v>
+      </c>
+      <c r="H42" s="21" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A43" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B43" s="8" t="s">
+      <c r="I42" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="J42" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="K42" s="21" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A43" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="B43" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="C43" s="10">
-        <v>0</v>
-      </c>
-      <c r="D43" s="10">
-        <v>0</v>
-      </c>
-      <c r="E43" s="10" t="s">
+      <c r="C43" s="21">
+        <v>0</v>
+      </c>
+      <c r="D43" s="21">
+        <v>0</v>
+      </c>
+      <c r="E43" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="F43" s="10">
-        <v>0</v>
-      </c>
-      <c r="G43" s="10">
-        <v>0</v>
-      </c>
-      <c r="H43" s="10" t="s">
+      <c r="F43" s="21">
+        <v>0</v>
+      </c>
+      <c r="G43" s="21">
+        <v>0</v>
+      </c>
+      <c r="H43" s="21" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A44" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B44" s="8" t="s">
+      <c r="I43" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="J43" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="K43" s="21" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A44" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="B44" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="C44" s="10">
+      <c r="C44" s="21">
         <v>9.1503269999999998E-2</v>
       </c>
-      <c r="D44" s="10">
+      <c r="D44" s="21">
         <v>0.60869565199999998</v>
       </c>
-      <c r="E44" s="10">
+      <c r="E44" s="21">
         <v>0.15909091</v>
       </c>
-      <c r="F44" s="10">
+      <c r="F44" s="21">
         <v>0.14285713999999999</v>
       </c>
-      <c r="G44" s="10">
+      <c r="G44" s="21">
         <v>0.30434782999999999</v>
       </c>
-      <c r="H44" s="10">
+      <c r="H44" s="21">
         <v>0.19444444</v>
       </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A45" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B45" s="8" t="s">
+      <c r="I44" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="J44" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="K44" s="21" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A45" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="B45" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="C45" s="10">
+      <c r="C45" s="21">
         <v>8.3333329999999997E-2</v>
       </c>
-      <c r="D45" s="10">
+      <c r="D45" s="21">
         <v>4.0540540999999999E-2</v>
       </c>
-      <c r="E45" s="10">
+      <c r="E45" s="21">
         <v>5.4545450000000002E-2</v>
       </c>
-      <c r="F45" s="10">
+      <c r="F45" s="21">
         <v>0.27272727000000002</v>
       </c>
-      <c r="G45" s="10">
+      <c r="G45" s="21">
         <v>0.24324324</v>
       </c>
-      <c r="H45" s="10">
+      <c r="H45" s="21">
         <v>0.25714285999999997</v>
       </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A46" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B46" s="8" t="s">
+      <c r="I45" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="J45" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="K45" s="21" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A46" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="B46" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="C46" s="10">
+      <c r="C46" s="21">
         <v>0.47096774000000002</v>
       </c>
-      <c r="D46" s="10">
+      <c r="D46" s="21">
         <v>0.544776119</v>
       </c>
-      <c r="E46" s="10">
+      <c r="E46" s="21">
         <v>0.50519031000000003</v>
       </c>
-      <c r="F46" s="10">
+      <c r="F46" s="21">
         <v>0.30801687999999999</v>
       </c>
-      <c r="G46" s="10">
+      <c r="G46" s="21">
         <v>0.54477611999999997</v>
       </c>
-      <c r="H46" s="10">
+      <c r="H46" s="21">
         <v>0.39353100000000002</v>
       </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A47" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B47" s="8" t="s">
+      <c r="I46" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="J46" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="K46" s="21" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A47" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="B47" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="C47" s="10">
+      <c r="C47" s="21">
         <v>0.11111111</v>
       </c>
-      <c r="D47" s="10">
+      <c r="D47" s="21">
         <v>6.3291140000000003E-3</v>
       </c>
-      <c r="E47" s="10">
+      <c r="E47" s="21">
         <v>1.197605E-2</v>
       </c>
-      <c r="F47" s="10">
-        <v>0</v>
-      </c>
-      <c r="G47" s="10">
-        <v>0</v>
-      </c>
-      <c r="H47" s="10" t="s">
+      <c r="F47" s="21">
+        <v>0</v>
+      </c>
+      <c r="G47" s="21">
+        <v>0</v>
+      </c>
+      <c r="H47" s="21" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A48" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B48" s="8" t="s">
+      <c r="I47" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="J47" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="K47" s="21" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A48" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="B48" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="C48" s="10">
-        <v>0</v>
-      </c>
-      <c r="D48" s="10">
-        <v>0</v>
-      </c>
-      <c r="E48" s="10" t="s">
+      <c r="C48" s="21">
+        <v>0</v>
+      </c>
+      <c r="D48" s="21">
+        <v>0</v>
+      </c>
+      <c r="E48" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="F48" s="10">
+      <c r="F48" s="21">
         <v>1.7543860000000001E-2</v>
       </c>
-      <c r="G48" s="10">
+      <c r="G48" s="21">
         <v>5.2631579999999997E-2</v>
       </c>
-      <c r="H48" s="10">
+      <c r="H48" s="21">
         <v>2.6315789999999999E-2</v>
       </c>
+      <c r="I48" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="J48" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="K48" s="21" t="s">
+        <v>18</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="12">
+    <mergeCell ref="I21:K21"/>
+    <mergeCell ref="G10:I10"/>
+    <mergeCell ref="G15:I15"/>
+    <mergeCell ref="A20:K20"/>
     <mergeCell ref="A41:B41"/>
     <mergeCell ref="A22:B22"/>
     <mergeCell ref="A10:C10"/>
@@ -4684,5 +7672,336 @@
     <mergeCell ref="F21:H21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D004AED-E3E1-164B-BD8A-552C264F9AAB}">
+  <dimension ref="A1:K13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21.6640625" customWidth="1"/>
+    <col min="2" max="2" width="21.83203125" customWidth="1"/>
+    <col min="5" max="5" width="15.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" s="35" t="s">
+        <v>100</v>
+      </c>
+      <c r="B1" s="35"/>
+    </row>
+    <row r="2" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+      <c r="A2" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="E2" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="27"/>
+      <c r="J2" s="27"/>
+      <c r="K2" s="27"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="15"/>
+      <c r="F3" s="32" t="s">
+        <v>103</v>
+      </c>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="36" t="s">
+        <v>49</v>
+      </c>
+      <c r="J3" s="36"/>
+      <c r="K3" s="36"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="34"/>
+      <c r="E4" s="22" t="s">
+        <v>104</v>
+      </c>
+      <c r="F4" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="J4" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="K4" s="18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="16">
+        <v>9.8214289999999996E-2</v>
+      </c>
+      <c r="G5" s="16">
+        <v>0.47826087</v>
+      </c>
+      <c r="H5" s="16">
+        <v>0.16296295999999999</v>
+      </c>
+      <c r="I5" s="18">
+        <v>0.2</v>
+      </c>
+      <c r="J5" s="18">
+        <v>0.21739130000000001</v>
+      </c>
+      <c r="K5" s="18">
+        <v>0.2083333</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="16">
+        <v>0.57563025000000001</v>
+      </c>
+      <c r="G6" s="16">
+        <v>0.72486771999999999</v>
+      </c>
+      <c r="H6" s="16">
+        <v>0.64168617999999999</v>
+      </c>
+      <c r="I6" s="18">
+        <v>0.57534249999999998</v>
+      </c>
+      <c r="J6" s="18">
+        <v>0.66666669999999995</v>
+      </c>
+      <c r="K6" s="18">
+        <v>0.6176471</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="34"/>
+      <c r="E7" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="16">
+        <v>0.25</v>
+      </c>
+      <c r="G7" s="16">
+        <v>1.3513509999999999E-2</v>
+      </c>
+      <c r="H7" s="16">
+        <v>2.5641029999999999E-2</v>
+      </c>
+      <c r="I7" s="18">
+        <v>0.24786320000000001</v>
+      </c>
+      <c r="J7" s="18">
+        <v>0.39189190000000002</v>
+      </c>
+      <c r="K7" s="18">
+        <v>0.30366490000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="34"/>
+      <c r="E8" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="16">
+        <v>0.51724137999999997</v>
+      </c>
+      <c r="G8" s="16">
+        <v>0.29032258</v>
+      </c>
+      <c r="H8" s="16">
+        <v>0.37190083000000002</v>
+      </c>
+      <c r="I8" s="18">
+        <v>0.47499999999999998</v>
+      </c>
+      <c r="J8" s="18">
+        <v>0.2451613</v>
+      </c>
+      <c r="K8" s="18">
+        <v>0.32340429999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="23" t="s">
+        <v>105</v>
+      </c>
+      <c r="F9" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="I9" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="J9" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="K9" s="24" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E10" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="21">
+        <v>0.1176471</v>
+      </c>
+      <c r="G10" s="21">
+        <v>0.43478260000000002</v>
+      </c>
+      <c r="H10" s="21">
+        <v>0.18518519999999999</v>
+      </c>
+      <c r="I10" s="24">
+        <v>0.15686269999999999</v>
+      </c>
+      <c r="J10" s="24">
+        <v>0.34782610000000003</v>
+      </c>
+      <c r="K10" s="24">
+        <v>0.2162162</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E11" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" s="21">
+        <v>0.65777779999999997</v>
+      </c>
+      <c r="G11" s="21">
+        <v>0.78306880000000001</v>
+      </c>
+      <c r="H11" s="21">
+        <v>0.71497580000000005</v>
+      </c>
+      <c r="I11" s="24">
+        <v>0.60173160000000003</v>
+      </c>
+      <c r="J11" s="24">
+        <v>0.73544969999999998</v>
+      </c>
+      <c r="K11" s="24">
+        <v>0.66190479999999996</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E12" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" s="21">
+        <v>0</v>
+      </c>
+      <c r="G12" s="21">
+        <v>0</v>
+      </c>
+      <c r="H12" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="I12" s="24">
+        <v>0.34</v>
+      </c>
+      <c r="J12" s="24">
+        <v>0.22972970000000001</v>
+      </c>
+      <c r="K12" s="24">
+        <v>0.27419349999999998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E13" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13" s="21">
+        <v>0.53846150000000004</v>
+      </c>
+      <c r="G13" s="21">
+        <v>0.45161289999999998</v>
+      </c>
+      <c r="H13" s="21">
+        <v>0.4912281</v>
+      </c>
+      <c r="I13" s="24">
+        <v>0.53211010000000003</v>
+      </c>
+      <c r="J13" s="24">
+        <v>0.37419350000000001</v>
+      </c>
+      <c r="K13" s="24">
+        <v>0.4393939</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="E2:K2"/>
+    <mergeCell ref="F3:H3"/>
+    <mergeCell ref="I3:K3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>